<commit_message>
xlsx com dados reais
</commit_message>
<xml_diff>
--- a/Project.xlsx
+++ b/Project.xlsx
@@ -4,25 +4,103 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Definitions" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Evidencias" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Word</t>
-  </si>
-  <si>
-    <t>Definition</t>
-  </si>
-  <si>
-    <t>Olá</t>
-  </si>
-  <si>
-    <t>Mundo</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Quantidade</t>
+  </si>
+  <si>
+    <t>Notas</t>
+  </si>
+  <si>
+    <t>Profundidade</t>
+  </si>
+  <si>
+    <t>Solo</t>
+  </si>
+  <si>
+    <t>Id do Ponto</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Status do Ponto</t>
+  </si>
+  <si>
+    <t>Usuário que criou</t>
+  </si>
+  <si>
+    <t>Usuário que atualizou</t>
+  </si>
+  <si>
+    <t>Data de criação</t>
+  </si>
+  <si>
+    <t>Data de atualização</t>
+  </si>
+  <si>
+    <t>"5dc8ab4637163e00178bd0e6"</t>
+  </si>
+  <si>
+    <t>Em aberto</t>
+  </si>
+  <si>
+    <t>Madeira</t>
+  </si>
+  <si>
+    <t>some fixed notes...</t>
+  </si>
+  <si>
+    <t>Superfície</t>
+  </si>
+  <si>
+    <t>Água</t>
+  </si>
+  <si>
+    <t>Realizado</t>
+  </si>
+  <si>
+    <t>"5d16de7d8db2ea00174a916a"</t>
+  </si>
+  <si>
+    <t>"5dc8aae737163e00178bd0e4"</t>
+  </si>
+  <si>
+    <t>20-30cm</t>
+  </si>
+  <si>
+    <t>Rocha</t>
+  </si>
+  <si>
+    <t>"5dc3065937a84c0017f7bd1a"</t>
+  </si>
+  <si>
+    <t>"5dcaaf0d50f17900176dff76"</t>
+  </si>
+  <si>
+    <t>10-20cm</t>
+  </si>
+  <si>
+    <t>"5dc75f42ea7b0500177d4381"</t>
   </si>
 </sst>
 </file>
@@ -58,8 +136,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,27 +478,234 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:O5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="36" customWidth="1"/>
-    <col min="2" max="2" width="120" customWidth="1"/>
+    <col min="2" max="15" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2">
+        <v>-45.9776900762719</v>
+      </c>
+      <c r="J2">
+        <v>-20.7172729395149</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="1">
+        <v>43775.04038826389</v>
+      </c>
+      <c r="O2" s="1">
+        <v>43780.01979832176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3">
+        <v>-46.0381655465671</v>
+      </c>
+      <c r="J3">
+        <v>-20.6904377923282</v>
+      </c>
+      <c r="K3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="1">
+        <v>43775.04038831018</v>
+      </c>
+      <c r="O3" s="1">
+        <v>43780.01895534722</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4">
+        <v>-46.0478527038117</v>
+      </c>
+      <c r="J4">
+        <v>-20.6878642170664</v>
+      </c>
+      <c r="K4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="1">
+        <v>43775.040388333335</v>
+      </c>
+      <c r="O4" s="1">
+        <v>43775.73864273148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5">
+        <v>-46.0308166248642</v>
+      </c>
+      <c r="J5">
+        <v>-20.6865044291569</v>
+      </c>
+      <c r="K5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5" s="1">
+        <v>43775.0403883449</v>
+      </c>
+      <c r="O5" s="1">
+        <v>43781.54820726852</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
xlsx com dados reais e consulta nova
</commit_message>
<xml_diff>
--- a/Project.xlsx
+++ b/Project.xlsx
@@ -11,12 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>Status</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
+  <si>
+    <t>Id da Evidência</t>
+  </si>
+  <si>
+    <t>Status da Evidência</t>
   </si>
   <si>
     <t>Tipo</t>
@@ -37,15 +37,24 @@
     <t>Id do Ponto</t>
   </si>
   <si>
-    <t>Longitude</t>
-  </si>
-  <si>
-    <t>Latitude</t>
+    <t>Nome do Ponto</t>
+  </si>
+  <si>
+    <t>Longitude do Ponto</t>
+  </si>
+  <si>
+    <t>Latitude do Ponto</t>
   </si>
   <si>
     <t>Status do Ponto</t>
   </si>
   <si>
+    <t>Id do Projeto</t>
+  </si>
+  <si>
+    <t>Nome do Projeto</t>
+  </si>
+  <si>
     <t>Usuário que criou</t>
   </si>
   <si>
@@ -76,10 +85,22 @@
     <t>Água</t>
   </si>
   <si>
+    <t>"5dc21aa103e32600176a26e6"</t>
+  </si>
+  <si>
+    <t>139</t>
+  </si>
+  <si>
     <t>Realizado</t>
   </si>
   <si>
-    <t>"5d16de7d8db2ea00174a916a"</t>
+    <t>"5dbf916a598a81001721843c"</t>
+  </si>
+  <si>
+    <t>Teste</t>
+  </si>
+  <si>
+    <t>Rodrigo Mota</t>
   </si>
   <si>
     <t>"5dc8aae737163e00178bd0e4"</t>
@@ -91,16 +112,34 @@
     <t>Rocha</t>
   </si>
   <si>
+    <t>"5dc21aa103e32600176a26ed"</t>
+  </si>
+  <si>
+    <t>146</t>
+  </si>
+  <si>
     <t>"5dc3065937a84c0017f7bd1a"</t>
   </si>
   <si>
+    <t>"5dc21aa103e32600176a26f0"</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
     <t>"5dcaaf0d50f17900176dff76"</t>
   </si>
   <si>
     <t>10-20cm</t>
   </si>
   <si>
-    <t>"5dc75f42ea7b0500177d4381"</t>
+    <t>"5dc21aa103e32600176a26f2"</t>
+  </si>
+  <si>
+    <t>151</t>
+  </si>
+  <si>
+    <t>Gustavo</t>
   </si>
 </sst>
 </file>
@@ -478,14 +517,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:R5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="36" customWidth="1"/>
-    <col min="2" max="15" width="50" customWidth="1"/>
+    <col min="1" max="3" width="30" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="80" customWidth="1"/>
+    <col min="6" max="8" width="30" customWidth="1"/>
+    <col min="9" max="9" width="50" customWidth="1"/>
+    <col min="10" max="10" width="320" customWidth="1"/>
+    <col min="11" max="18" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -531,180 +575,237 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2">
+        <v>-45.9776900762719</v>
+      </c>
+      <c r="K2">
+        <v>-20.7172729395149</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>43775.04038826389</v>
+      </c>
+      <c r="R2" s="1">
+        <v>43780.01979832176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="G2" t="s">
+      <c r="C3" t="s">
         <v>20</v>
-      </c>
-      <c r="I2">
-        <v>-45.9776900762719</v>
-      </c>
-      <c r="J2">
-        <v>-20.7172729395149</v>
-      </c>
-      <c r="K2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="1">
-        <v>43775.04038826389</v>
-      </c>
-      <c r="O2" s="1">
-        <v>43780.01979832176</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3">
+        <v>32</v>
+      </c>
+      <c r="H3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3">
         <v>-46.0381655465671</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>-20.6904377923282</v>
       </c>
-      <c r="K3" t="s">
-        <v>21</v>
-      </c>
       <c r="L3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="M3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N3" s="1">
+        <v>27</v>
+      </c>
+      <c r="N3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" s="1">
         <v>43775.04038831018</v>
       </c>
-      <c r="O3" s="1">
+      <c r="R3" s="1">
         <v>43780.01895534722</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4">
+        <v>-46.0478527038117</v>
+      </c>
+      <c r="K4">
+        <v>-20.6878642170664</v>
+      </c>
+      <c r="L4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" t="s">
+        <v>29</v>
+      </c>
+      <c r="P4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>43775.040388333335</v>
+      </c>
+      <c r="R4" s="1">
+        <v>43775.73864273148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="G4" t="s">
+      <c r="C5" t="s">
         <v>20</v>
-      </c>
-      <c r="I4">
-        <v>-46.0478527038117</v>
-      </c>
-      <c r="J4">
-        <v>-20.6878642170664</v>
-      </c>
-      <c r="K4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N4" s="1">
-        <v>43775.040388333335</v>
-      </c>
-      <c r="O4" s="1">
-        <v>43775.73864273148</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5">
+        <v>-46.0308166248642</v>
+      </c>
+      <c r="K5">
+        <v>-20.6865044291569</v>
+      </c>
+      <c r="L5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" t="s">
         <v>28</v>
       </c>
-      <c r="G5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5">
-        <v>-46.0308166248642</v>
-      </c>
-      <c r="J5">
-        <v>-20.6865044291569</v>
-      </c>
-      <c r="K5" t="s">
-        <v>21</v>
-      </c>
-      <c r="L5" t="s">
-        <v>22</v>
-      </c>
-      <c r="M5" t="s">
+      <c r="O5" t="s">
         <v>29</v>
       </c>
-      <c r="N5" s="1">
+      <c r="P5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q5" s="1">
         <v>43775.0403883449</v>
       </c>
-      <c r="O5" s="1">
+      <c r="R5" s="1">
         <v>43781.54820726852</v>
       </c>
     </row>

</xml_diff>